<commit_message>
can now use many banks in each bank.txt and fixed link bug
</commit_message>
<xml_diff>
--- a/todaysBank.xlsx
+++ b/todaysBank.xlsx
@@ -34,10 +34,10 @@
     <t>Aegis of Stormwind</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=1203) </t>
-  </si>
-  <si>
-    <t>peanuts</t>
+    <t>https://database.turtle-wow.org/?item=1203</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
   </si>
   <si>
     <t>20</t>
@@ -46,7 +46,7 @@
     <t>Aquamarine</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7909) </t>
+    <t>https://database.turtle-wow.org/?item=7909</t>
   </si>
   <si>
     <t>40</t>
@@ -55,31 +55,31 @@
     <t>Arcane Crystal</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12363) </t>
+    <t>https://database.turtle-wow.org/?item=12363</t>
   </si>
   <si>
     <t>Arcanite Bar</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12360) </t>
+    <t>https://database.turtle-wow.org/?item=12360</t>
   </si>
   <si>
     <t>Azerothian Diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12800) </t>
+    <t>https://database.turtle-wow.org/?item=12800</t>
   </si>
   <si>
     <t>Belt of Valor</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16736) </t>
+    <t>https://database.turtle-wow.org/?item=16736</t>
   </si>
   <si>
     <t>Black Diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11754) </t>
+    <t>https://database.turtle-wow.org/?item=11754</t>
   </si>
   <si>
     <t>8</t>
@@ -88,13 +88,13 @@
     <t>Black Lotus</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13468) </t>
+    <t>https://database.turtle-wow.org/?item=13468</t>
   </si>
   <si>
     <t>Black Pearl</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7971) </t>
+    <t>https://database.turtle-wow.org/?item=7971</t>
   </si>
   <si>
     <t>4</t>
@@ -103,13 +103,13 @@
     <t>Blood of the Mountain</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11382) </t>
+    <t>https://database.turtle-wow.org/?item=11382</t>
   </si>
   <si>
     <t>Blue Sapphire</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12361) </t>
+    <t>https://database.turtle-wow.org/?item=12361</t>
   </si>
   <si>
     <t>2</t>
@@ -118,13 +118,13 @@
     <t>Book: Gift of the Wild</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=17682) </t>
+    <t>https://database.turtle-wow.org/?item=17682</t>
   </si>
   <si>
     <t>Book: Gift of the Wild II</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=17683) </t>
+    <t>https://database.turtle-wow.org/?item=17683</t>
   </si>
   <si>
     <t>9</t>
@@ -133,31 +133,31 @@
     <t>Breath of Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7081) </t>
+    <t>https://database.turtle-wow.org/?item=7081</t>
   </si>
   <si>
     <t>Brilliant Chromatic Scale</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12607) </t>
+    <t>https://database.turtle-wow.org/?item=12607</t>
   </si>
   <si>
     <t>Burning War Axe</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=2299) </t>
+    <t>https://database.turtle-wow.org/?item=2299</t>
   </si>
   <si>
     <t>Cassandra's Grace</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13102) </t>
+    <t>https://database.turtle-wow.org/?item=13102</t>
   </si>
   <si>
     <t>Codex: Prayer of Fortitude II</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=17414) </t>
+    <t>https://database.turtle-wow.org/?item=17414</t>
   </si>
   <si>
     <t>3</t>
@@ -166,19 +166,19 @@
     <t>Codex: Prayer of Shadow Protection</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=22393) </t>
+    <t>https://database.turtle-wow.org/?item=22393</t>
   </si>
   <si>
     <t>Core of Earth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7075) </t>
+    <t>https://database.turtle-wow.org/?item=7075</t>
   </si>
   <si>
     <t>Cow King's Hide</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13009) </t>
+    <t>https://database.turtle-wow.org/?item=13009</t>
   </si>
   <si>
     <t>11</t>
@@ -187,7 +187,7 @@
     <t>Dark Iron Bar</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11371) </t>
+    <t>https://database.turtle-wow.org/?item=11371</t>
   </si>
   <si>
     <t>481</t>
@@ -196,7 +196,7 @@
     <t>Dark Iron Residue</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=18945) </t>
+    <t>https://database.turtle-wow.org/?item=18945</t>
   </si>
   <si>
     <t>15</t>
@@ -205,91 +205,91 @@
     <t>Dense Sharpening Stone</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12404) </t>
+    <t>https://database.turtle-wow.org/?item=12404</t>
   </si>
   <si>
     <t>Destiny</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=647) </t>
+    <t>https://database.turtle-wow.org/?item=647</t>
   </si>
   <si>
     <t>Devout Belt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16696) </t>
+    <t>https://database.turtle-wow.org/?item=16696</t>
   </si>
   <si>
     <t>Devout Gloves</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16692) </t>
+    <t>https://database.turtle-wow.org/?item=16692</t>
   </si>
   <si>
     <t>Discombobulator Ray</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=4388) </t>
+    <t>https://database.turtle-wow.org/?item=4388</t>
   </si>
   <si>
     <t>Dreadmist Belt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16702) </t>
+    <t>https://database.turtle-wow.org/?item=16702</t>
   </si>
   <si>
     <t>Dreamfoil</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13463) </t>
+    <t>https://database.turtle-wow.org/?item=13463</t>
   </si>
   <si>
     <t>Edgemaster's Handguards</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14551) </t>
+    <t>https://database.turtle-wow.org/?item=14551</t>
   </si>
   <si>
     <t>Eidolon Talisman</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=18340) </t>
+    <t>https://database.turtle-wow.org/?item=18340</t>
   </si>
   <si>
     <t>Eight of Beasts</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19236) </t>
+    <t>https://database.turtle-wow.org/?item=19236</t>
   </si>
   <si>
     <t>Elder Wizard's Mantle</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13013) </t>
+    <t>https://database.turtle-wow.org/?item=13013</t>
   </si>
   <si>
     <t>Elemental Air</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7069) </t>
+    <t>https://database.turtle-wow.org/?item=7069</t>
   </si>
   <si>
     <t>Elemental Earth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7067) </t>
+    <t>https://database.turtle-wow.org/?item=7067</t>
   </si>
   <si>
     <t>Elemental Fire</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7068) </t>
+    <t>https://database.turtle-wow.org/?item=7068</t>
   </si>
   <si>
     <t>Elemental Water</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7070) </t>
+    <t>https://database.turtle-wow.org/?item=7070</t>
   </si>
   <si>
     <t>43</t>
@@ -298,25 +298,25 @@
     <t>Essence of Air</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7082) </t>
+    <t>https://database.turtle-wow.org/?item=7082</t>
   </si>
   <si>
     <t>Essence of Earth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7076) </t>
+    <t>https://database.turtle-wow.org/?item=7076</t>
   </si>
   <si>
     <t>Essence of Fire</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7078) </t>
+    <t>https://database.turtle-wow.org/?item=7078</t>
   </si>
   <si>
     <t>Essence of Undeath</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12808) </t>
+    <t>https://database.turtle-wow.org/?item=12808</t>
   </si>
   <si>
     <t>10</t>
@@ -325,67 +325,67 @@
     <t>Essence of Water</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7080) </t>
+    <t>https://database.turtle-wow.org/?item=7080</t>
   </si>
   <si>
     <t>Five of Beasts</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19233) </t>
+    <t>https://database.turtle-wow.org/?item=19233</t>
   </si>
   <si>
     <t>Foror's Compendium of Dragon Slaying</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=18401) </t>
+    <t>https://database.turtle-wow.org/?item=18401</t>
   </si>
   <si>
     <t>Four of Beasts</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19232) </t>
+    <t>https://database.turtle-wow.org/?item=19232</t>
   </si>
   <si>
     <t>Frenzied Striker</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13056) </t>
+    <t>https://database.turtle-wow.org/?item=13056</t>
   </si>
   <si>
     <t>Globe of Water</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7079) </t>
+    <t>https://database.turtle-wow.org/?item=7079</t>
   </si>
   <si>
     <t>Golden Pearl</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13926) </t>
+    <t>https://database.turtle-wow.org/?item=13926</t>
   </si>
   <si>
     <t>Golden Rod</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11128) </t>
+    <t>https://database.turtle-wow.org/?item=11128</t>
   </si>
   <si>
     <t>Grimoire of Shadow Ward IV</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=22891) </t>
+    <t>https://database.turtle-wow.org/?item=22891</t>
   </si>
   <si>
     <t>Gromsblood</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=8846) </t>
+    <t>https://database.turtle-wow.org/?item=8846</t>
   </si>
   <si>
     <t>Gut Ripper</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=2164) </t>
+    <t>https://database.turtle-wow.org/?item=2164</t>
   </si>
   <si>
     <t>6</t>
@@ -394,7 +394,7 @@
     <t>Heart of Fire</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=7077) </t>
+    <t>https://database.turtle-wow.org/?item=7077</t>
   </si>
   <si>
     <t>29</t>
@@ -403,277 +403,277 @@
     <t>Heart of the Wild</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=10286) </t>
+    <t>https://database.turtle-wow.org/?item=10286</t>
   </si>
   <si>
     <t>Huge Emerald</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12364) </t>
+    <t>https://database.turtle-wow.org/?item=12364</t>
   </si>
   <si>
     <t>Ironweb Spider Silk</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14227) </t>
+    <t>https://database.turtle-wow.org/?item=14227</t>
   </si>
   <si>
     <t>Jade</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=1529) </t>
+    <t>https://database.turtle-wow.org/?item=1529</t>
   </si>
   <si>
     <t>Kang the Decapitator</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=2291) </t>
+    <t>https://database.turtle-wow.org/?item=2291</t>
   </si>
   <si>
     <t>Large Opal</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12799) </t>
+    <t>https://database.turtle-wow.org/?item=12799</t>
   </si>
   <si>
     <t>Lightforge Belt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16723) </t>
+    <t>https://database.turtle-wow.org/?item=16723</t>
   </si>
   <si>
     <t>Lord Alexander's Battle Axe</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13003) </t>
+    <t>https://database.turtle-wow.org/?item=13003</t>
   </si>
   <si>
     <t>Mageweave Cloth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=4338) </t>
+    <t>https://database.turtle-wow.org/?item=4338</t>
   </si>
   <si>
     <t>Magician's Mantle</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12998) </t>
+    <t>https://database.turtle-wow.org/?item=12998</t>
   </si>
   <si>
     <t>Magister's Belt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16685) </t>
+    <t>https://database.turtle-wow.org/?item=16685</t>
   </si>
   <si>
     <t>Major Mana Potion</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13444) </t>
+    <t>https://database.turtle-wow.org/?item=13444</t>
   </si>
   <si>
     <t>Medallion of Grand Marshal Morris</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13091) </t>
+    <t>https://database.turtle-wow.org/?item=13091</t>
   </si>
   <si>
     <t>Mooncloth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14342) </t>
+    <t>https://database.turtle-wow.org/?item=14342</t>
   </si>
   <si>
     <t>Moss Agate</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=1206) </t>
+    <t>https://database.turtle-wow.org/?item=1206</t>
   </si>
   <si>
     <t>Mountain Silversage</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13465) </t>
+    <t>https://database.turtle-wow.org/?item=13465</t>
   </si>
   <si>
     <t>Obsidian Greaves</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13068) </t>
+    <t>https://database.turtle-wow.org/?item=13068</t>
   </si>
   <si>
     <t>Oily Blackmouth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=6358) </t>
+    <t>https://database.turtle-wow.org/?item=6358</t>
   </si>
   <si>
     <t>Pads of the Venom Spider</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13103) </t>
+    <t>https://database.turtle-wow.org/?item=13103</t>
   </si>
   <si>
     <t>Pattern: Black Dragonscale Shoulders</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=15770) </t>
+    <t>https://database.turtle-wow.org/?item=15770</t>
   </si>
   <si>
     <t>Pattern: Living Leggings</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=15752) </t>
+    <t>https://database.turtle-wow.org/?item=15752</t>
   </si>
   <si>
     <t>Pattern: Robe of the Archmage</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14513) </t>
+    <t>https://database.turtle-wow.org/?item=14513</t>
   </si>
   <si>
     <t>Pattern: Robe of the Void</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14514) </t>
+    <t>https://database.turtle-wow.org/?item=14514</t>
   </si>
   <si>
     <t>Plans: Annihilator</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12835) </t>
+    <t>https://database.turtle-wow.org/?item=12835</t>
   </si>
   <si>
     <t>Plans: Invulnerable Mail</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12728) </t>
+    <t>https://database.turtle-wow.org/?item=12728</t>
   </si>
   <si>
     <t>Plans: Rune-Etched Crown</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=83504) </t>
+    <t>https://database.turtle-wow.org/?item=83504</t>
   </si>
   <si>
     <t>Plans: Rune-Etched Greaves</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=83501) </t>
+    <t>https://database.turtle-wow.org/?item=83501</t>
   </si>
   <si>
     <t>Plans: Rune-Etched Grips</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=83506) </t>
+    <t>https://database.turtle-wow.org/?item=83506</t>
   </si>
   <si>
     <t>Plans: Rune-Etched Mantle</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=83505) </t>
+    <t>https://database.turtle-wow.org/?item=83505</t>
   </si>
   <si>
     <t>Plans: Storm Gauntlets</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12703) </t>
+    <t>https://database.turtle-wow.org/?item=12703</t>
   </si>
   <si>
     <t>Plans: Untempered Runeblade</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=83500) </t>
+    <t>https://database.turtle-wow.org/?item=83500</t>
   </si>
   <si>
     <t>Pristine Black Diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=18335) </t>
+    <t>https://database.turtle-wow.org/?item=18335</t>
   </si>
   <si>
     <t>Quickdraw Quiver</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=8217) </t>
+    <t>https://database.turtle-wow.org/?item=8217</t>
   </si>
   <si>
     <t>Recipe: Greater Frost Protection Potion</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13495) </t>
+    <t>https://database.turtle-wow.org/?item=13495</t>
   </si>
   <si>
     <t>Ribsplitter of Stamina</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12527) </t>
+    <t>https://database.turtle-wow.org/?item=12527</t>
   </si>
   <si>
     <t>Righteous Orb</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12811) </t>
+    <t>https://database.turtle-wow.org/?item=12811</t>
   </si>
   <si>
     <t>Rugged Leather</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=8170) </t>
+    <t>https://database.turtle-wow.org/?item=8170</t>
   </si>
   <si>
     <t>Runecloth</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=14047) </t>
+    <t>https://database.turtle-wow.org/?item=14047</t>
   </si>
   <si>
     <t>Sandals of the Insurgent</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13111) </t>
+    <t>https://database.turtle-wow.org/?item=13111</t>
   </si>
   <si>
     <t>Schematic: Sniper Scope</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=10608) </t>
+    <t>https://database.turtle-wow.org/?item=10608</t>
   </si>
   <si>
     <t>Seven of Warlords</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19264) </t>
+    <t>https://database.turtle-wow.org/?item=19264</t>
   </si>
   <si>
     <t>Six of Beasts</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19234) </t>
+    <t>https://database.turtle-wow.org/?item=19234</t>
   </si>
   <si>
     <t>Six of Warlords</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19263) </t>
+    <t>https://database.turtle-wow.org/?item=19263</t>
   </si>
   <si>
     <t>Small Flame Sac</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=4402) </t>
+    <t>https://database.turtle-wow.org/?item=4402</t>
   </si>
   <si>
     <t>Small Glowing Shard</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11138) </t>
+    <t>https://database.turtle-wow.org/?item=11138</t>
   </si>
   <si>
     <t>Spaulders of the Unseen</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13116) </t>
+    <t>https://database.turtle-wow.org/?item=13116</t>
   </si>
   <si>
     <t>162</t>
@@ -682,7 +682,7 @@
     <t>Stonescale Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13423) </t>
+    <t>https://database.turtle-wow.org/?item=13423</t>
   </si>
   <si>
     <t>12</t>
@@ -691,103 +691,103 @@
     <t>Stranglekelp</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=3820) </t>
+    <t>https://database.turtle-wow.org/?item=3820</t>
   </si>
   <si>
     <t>Teebu's Blazing Longsword</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=1728) </t>
+    <t>https://database.turtle-wow.org/?item=1728</t>
   </si>
   <si>
     <t>The Judge's Gavel</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=12528) </t>
+    <t>https://database.turtle-wow.org/?item=12528</t>
   </si>
   <si>
     <t>The Ziggler</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=8006) </t>
+    <t>https://database.turtle-wow.org/?item=8006</t>
   </si>
   <si>
     <t>Thick Leather</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=4304) </t>
+    <t>https://database.turtle-wow.org/?item=4304</t>
   </si>
   <si>
     <t>Three of Warlords</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19260) </t>
+    <t>https://database.turtle-wow.org/?item=19260</t>
   </si>
   <si>
     <t>Tome of Arcane Brilliance</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=18600) </t>
+    <t>https://database.turtle-wow.org/?item=18600</t>
   </si>
   <si>
     <t>Tome of Conjure Food VII</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=22897) </t>
+    <t>https://database.turtle-wow.org/?item=22897</t>
   </si>
   <si>
     <t>Tome of Frost Ward V</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=22890) </t>
+    <t>https://database.turtle-wow.org/?item=22890</t>
   </si>
   <si>
     <t>Traveler's Backpack</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=4500) </t>
+    <t>https://database.turtle-wow.org/?item=4500</t>
   </si>
   <si>
     <t>Truesilver Rod</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=11144) </t>
+    <t>https://database.turtle-wow.org/?item=11144</t>
   </si>
   <si>
     <t>Two of Beasts</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19230) </t>
+    <t>https://database.turtle-wow.org/?item=19230</t>
   </si>
   <si>
     <t>Two of Warlords</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=19259) </t>
+    <t>https://database.turtle-wow.org/?item=19259</t>
   </si>
   <si>
     <t>Volatile Rum</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=9260) </t>
+    <t>https://database.turtle-wow.org/?item=9260</t>
   </si>
   <si>
     <t>Wildheart Bracers</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=16714) </t>
+    <t>https://database.turtle-wow.org/?item=16714</t>
   </si>
   <si>
     <t>Winged Helm</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=13112) </t>
+    <t>https://database.turtle-wow.org/?item=13112</t>
   </si>
   <si>
     <t>Wirt's Third Leg</t>
   </si>
   <si>
-    <t xml:space="preserve">https://database.turtle-wow.org/?item=9359) </t>
+    <t>https://database.turtle-wow.org/?item=9359</t>
   </si>
   <si>
     <t>DDMMYYYY 20-2-2023</t>

</xml_diff>